<commit_message>
employees statistics section add
</commit_message>
<xml_diff>
--- a/excel/employees_balance.xlsx
+++ b/excel/employees_balance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS-Services.Uz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS-Services.Uz\Desktop\mebel.akmalovich.uz\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C5CF00-1CC1-4E5A-B386-81CD9DE1716D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52976C88-F58C-4958-82E0-85A32FDE2440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C06EB67F-69BB-42A5-BBC2-969FBFB13C86}"/>
   </bookViews>
@@ -158,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,16 +205,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -222,23 +235,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -259,10 +282,23 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
+    <cellStyle name="Хороший" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -665,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E53139-E54A-46D2-9994-8B7D2D9967EC}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,754 +720,754 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="10">
         <v>46054</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11">
         <v>50000</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="11">
         <v>25000</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10">
         <v>46055</v>
       </c>
-      <c r="G2" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="G2" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="10">
         <v>46055</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1" t="e" vm="1">
+      <c r="B3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="I3" s="1" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="10">
         <v>46056</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J4" s="8">
+      <c r="B4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J4" s="6">
         <v>2022</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="10">
         <v>46057</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J5" s="8">
+      <c r="B5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J5" s="6">
         <v>2023</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="10">
         <v>46058</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J6" s="8">
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" s="6">
         <v>2024</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="10">
         <v>46059</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11">
         <v>150000</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="11">
         <v>10000</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="10">
         <v>46059</v>
       </c>
-      <c r="G7" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J7" s="8">
+      <c r="G7" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J7" s="6">
         <v>2025</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="10">
         <v>46060</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J8" s="8">
+      <c r="B8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J8" s="6">
         <v>2026</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="10">
         <v>46061</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J9" s="8"/>
+      <c r="B9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="10">
         <v>46062</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="1" t="e" vm="1">
+      <c r="B10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="I10" s="2" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="10">
         <v>46063</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="1" t="e" vm="1">
+      <c r="B11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="10">
         <v>46064</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="1" t="e" vm="1">
+      <c r="B12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="10">
         <v>46065</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1" t="e" vm="1">
+      <c r="B13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="10">
         <v>46066</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1" t="e" vm="1">
+      <c r="B14" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="10">
         <v>46067</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="1" t="e" vm="1">
+      <c r="B15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="10">
         <v>46068</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J16" s="9" t="s">
+      <c r="B16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J16" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="10">
         <v>46069</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J17" s="9" t="s">
+      <c r="B17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J17" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="10">
         <v>46070</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J18" s="9" t="s">
+      <c r="B18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="10">
         <v>46071</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J19" s="9" t="s">
+      <c r="B19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="10">
         <v>46072</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J20" s="9" t="s">
+      <c r="B20" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="10">
         <v>46073</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J21" s="9" t="s">
+      <c r="B21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="11">
+        <v>0</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J21" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="10">
         <v>46074</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0</v>
-      </c>
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J22" s="8"/>
+      <c r="B22" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="10">
         <v>46075</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I23" s="5" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J23" s="7" t="s">
+      <c r="B23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I23" s="3" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="10">
         <v>46076</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J24" s="10" t="s">
+      <c r="B24" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J24" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="10">
         <v>46077</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4">
-        <v>0</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J25" s="10" t="s">
+      <c r="B25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0</v>
+      </c>
+      <c r="D25" s="11">
+        <v>0</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J25" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="10">
         <v>46078</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4">
-        <v>0</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="1" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J26" s="10" t="s">
+      <c r="B26" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0</v>
+      </c>
+      <c r="D26" s="11">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J26" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="10">
         <v>46079</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="1" t="e" vm="1">
+      <c r="B27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0</v>
+      </c>
+      <c r="D27" s="11">
+        <v>0</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="A28" s="10">
         <v>46080</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="1" t="e" vm="1">
+      <c r="B28" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="A29" s="10">
         <v>46081</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" s="1" t="e" vm="1">
+      <c r="B29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>